<commit_message>
fix: small bugs in data loading/testing
</commit_message>
<xml_diff>
--- a/tests/datasets/test_mix_labels.xlsx
+++ b/tests/datasets/test_mix_labels.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
   <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
     <t xml:space="preserve">label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aa</t>
   </si>
   <si>
     <t xml:space="preserve">a</t>
@@ -116,8 +119,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -141,165 +148,168 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="0" t="n">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="0" t="n">
+      <c r="A15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="0" t="n">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="0" t="n">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="0" t="n">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="0" t="n">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="0" t="n">
+      <c r="A20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="1" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>